<commit_message>
Updated excel with data from 3/23/2020
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C069845-80B0-514A-85E6-1B6D78CA39E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D5C5AA1-DDE7-0E44-BDC7-5C50E468BBC5}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1140" windowWidth="24860" windowHeight="9740"/>
+    <workbookView xWindow="500" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -114,11 +114,14 @@
   <si>
     <t>Wharton</t>
   </si>
+  <si>
+    <t>10-20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -599,7 +602,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -954,12 +957,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F143"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E181" sqref="E181"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1211,8 +1220,8 @@
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="2">
-        <v>44124</v>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -2978,8 +2987,8 @@
       <c r="B130" t="s">
         <v>11</v>
       </c>
-      <c r="C130" s="2">
-        <v>44124</v>
+      <c r="C130" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D130" t="s">
         <v>10</v>
@@ -3171,6 +3180,667 @@
       </c>
       <c r="D143" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B144" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" t="s">
+        <v>20</v>
+      </c>
+      <c r="E144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" t="s">
+        <v>19</v>
+      </c>
+      <c r="D145" t="s">
+        <v>10</v>
+      </c>
+      <c r="E145" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B146" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" t="s">
+        <v>18</v>
+      </c>
+      <c r="D146" t="s">
+        <v>10</v>
+      </c>
+      <c r="E146" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" t="s">
+        <v>10</v>
+      </c>
+      <c r="E147" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" t="s">
+        <v>17</v>
+      </c>
+      <c r="D148" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" t="s">
+        <v>10</v>
+      </c>
+      <c r="E149" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" t="s">
+        <v>19</v>
+      </c>
+      <c r="D150" t="s">
+        <v>13</v>
+      </c>
+      <c r="E150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" t="s">
+        <v>15</v>
+      </c>
+      <c r="E151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" t="s">
+        <v>15</v>
+      </c>
+      <c r="E152" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B153" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" t="s">
+        <v>20</v>
+      </c>
+      <c r="E153" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B154" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" t="s">
+        <v>17</v>
+      </c>
+      <c r="D154" t="s">
+        <v>20</v>
+      </c>
+      <c r="E154" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B155" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D155" t="s">
+        <v>20</v>
+      </c>
+      <c r="E155" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>43912</v>
+      </c>
+      <c r="D156" t="s">
+        <v>22</v>
+      </c>
+      <c r="E156" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>43912</v>
+      </c>
+      <c r="D157" t="s">
+        <v>22</v>
+      </c>
+      <c r="E157" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D158" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D164" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D165" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D166" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D167" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D168" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D169" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D170" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171" t="s">
+        <v>12</v>
+      </c>
+      <c r="D171" t="s">
+        <v>24</v>
+      </c>
+      <c r="E171" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172" t="s">
+        <v>19</v>
+      </c>
+      <c r="D172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B173" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" t="s">
+        <v>28</v>
+      </c>
+      <c r="D173" t="s">
+        <v>20</v>
+      </c>
+      <c r="E173" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B174" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D174" t="s">
+        <v>15</v>
+      </c>
+      <c r="E174" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B175" t="s">
+        <v>11</v>
+      </c>
+      <c r="C175" t="s">
+        <v>17</v>
+      </c>
+      <c r="D175" t="s">
+        <v>15</v>
+      </c>
+      <c r="E175" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" t="s">
+        <v>18</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
+        <v>18</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+      <c r="E177" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B178" t="s">
+        <v>11</v>
+      </c>
+      <c r="C178" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B179" t="s">
+        <v>11</v>
+      </c>
+      <c r="C179" t="s">
+        <v>12</v>
+      </c>
+      <c r="D179" t="s">
+        <v>10</v>
+      </c>
+      <c r="E179" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" t="s">
+        <v>18</v>
+      </c>
+      <c r="D180" t="s">
+        <v>10</v>
+      </c>
+      <c r="E180" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
+        <v>17</v>
+      </c>
+      <c r="D181" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" t="s">
+        <v>18</v>
+      </c>
+      <c r="D182" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" t="s">
+        <v>17</v>
+      </c>
+      <c r="D183" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B184" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" t="s">
+        <v>17</v>
+      </c>
+      <c r="D184" t="s">
+        <v>20</v>
+      </c>
+      <c r="E184" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B185" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185" t="s">
+        <v>17</v>
+      </c>
+      <c r="D185" t="s">
+        <v>20</v>
+      </c>
+      <c r="E185" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B186" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" t="s">
+        <v>20</v>
+      </c>
+      <c r="E186" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" t="s">
+        <v>18</v>
+      </c>
+      <c r="D187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E187" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188" t="s">
+        <v>12</v>
+      </c>
+      <c r="D188" t="s">
+        <v>20</v>
+      </c>
+      <c r="E188" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B189" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189" t="s">
+        <v>17</v>
+      </c>
+      <c r="D189" t="s">
+        <v>24</v>
+      </c>
+      <c r="E189" t="s">
+        <v>16</v>
+      </c>
+      <c r="F189" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" t="s">
+        <v>18</v>
+      </c>
+      <c r="D190" t="s">
+        <v>24</v>
+      </c>
+      <c r="E190" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added numbers from 3/24
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D5C5AA1-DDE7-0E44-BDC7-5C50E468BBC5}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFC3F3DF-13C0-1D43-84A0-5AED8A9D1873}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -599,10 +599,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -958,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3843,6 +3844,998 @@
         <v>16</v>
       </c>
     </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D191" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D192" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D194" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D196" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B197" t="s">
+        <v>11</v>
+      </c>
+      <c r="C197" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" t="s">
+        <v>24</v>
+      </c>
+      <c r="E197" t="s">
+        <v>16</v>
+      </c>
+      <c r="F197" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B198" t="s">
+        <v>11</v>
+      </c>
+      <c r="C198" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" t="s">
+        <v>24</v>
+      </c>
+      <c r="E198" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B199" t="s">
+        <v>11</v>
+      </c>
+      <c r="C199" t="s">
+        <v>19</v>
+      </c>
+      <c r="D199" t="s">
+        <v>24</v>
+      </c>
+      <c r="E199" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B200" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200" t="s">
+        <v>18</v>
+      </c>
+      <c r="D200" t="s">
+        <v>24</v>
+      </c>
+      <c r="E200" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B201" t="s">
+        <v>11</v>
+      </c>
+      <c r="C201" t="s">
+        <v>19</v>
+      </c>
+      <c r="D201" t="s">
+        <v>24</v>
+      </c>
+      <c r="F201" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B202" t="s">
+        <v>11</v>
+      </c>
+      <c r="C202" t="s">
+        <v>19</v>
+      </c>
+      <c r="D202" t="s">
+        <v>24</v>
+      </c>
+      <c r="F202" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B203" t="s">
+        <v>11</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D203" t="s">
+        <v>24</v>
+      </c>
+      <c r="F203" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B204" t="s">
+        <v>11</v>
+      </c>
+      <c r="C204" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B205" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" t="s">
+        <v>17</v>
+      </c>
+      <c r="D205" t="s">
+        <v>24</v>
+      </c>
+      <c r="F205" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B206" t="s">
+        <v>11</v>
+      </c>
+      <c r="C206" t="s">
+        <v>18</v>
+      </c>
+      <c r="D206" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B207" t="s">
+        <v>11</v>
+      </c>
+      <c r="C207" t="s">
+        <v>25</v>
+      </c>
+      <c r="D207" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B208" t="s">
+        <v>11</v>
+      </c>
+      <c r="C208" t="s">
+        <v>18</v>
+      </c>
+      <c r="D208" t="s">
+        <v>20</v>
+      </c>
+      <c r="E208" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B209" t="s">
+        <v>11</v>
+      </c>
+      <c r="C209" t="s">
+        <v>17</v>
+      </c>
+      <c r="D209" t="s">
+        <v>20</v>
+      </c>
+      <c r="E209" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" t="s">
+        <v>18</v>
+      </c>
+      <c r="D210" t="s">
+        <v>20</v>
+      </c>
+      <c r="E210" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D211" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D212" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D213" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D214" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D215" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D216" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D217" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D218" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D219" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D220" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D221" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D222" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D223" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D224" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D225" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D226" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D227" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D228" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D230" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D231" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D232" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D233" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D234" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D235" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D236" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D237" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D238" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D239" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D240" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D241" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B242" t="s">
+        <v>11</v>
+      </c>
+      <c r="D242" t="s">
+        <v>10</v>
+      </c>
+      <c r="E242" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B243" t="s">
+        <v>11</v>
+      </c>
+      <c r="D243" t="s">
+        <v>10</v>
+      </c>
+      <c r="E243" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B244" t="s">
+        <v>11</v>
+      </c>
+      <c r="D244" t="s">
+        <v>10</v>
+      </c>
+      <c r="E244" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B245" t="s">
+        <v>11</v>
+      </c>
+      <c r="D245" t="s">
+        <v>10</v>
+      </c>
+      <c r="E245" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B246" t="s">
+        <v>11</v>
+      </c>
+      <c r="D246" t="s">
+        <v>10</v>
+      </c>
+      <c r="E246" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B247" t="s">
+        <v>11</v>
+      </c>
+      <c r="D247" t="s">
+        <v>10</v>
+      </c>
+      <c r="E247" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B248" t="s">
+        <v>11</v>
+      </c>
+      <c r="D248" t="s">
+        <v>10</v>
+      </c>
+      <c r="E248" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B249" t="s">
+        <v>11</v>
+      </c>
+      <c r="D249" t="s">
+        <v>10</v>
+      </c>
+      <c r="E249" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B250" t="s">
+        <v>11</v>
+      </c>
+      <c r="D250" t="s">
+        <v>10</v>
+      </c>
+      <c r="E250" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B251" t="s">
+        <v>11</v>
+      </c>
+      <c r="D251" t="s">
+        <v>10</v>
+      </c>
+      <c r="E251" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B252" t="s">
+        <v>11</v>
+      </c>
+      <c r="D252" t="s">
+        <v>10</v>
+      </c>
+      <c r="E252" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B253" t="s">
+        <v>6</v>
+      </c>
+      <c r="D253" t="s">
+        <v>10</v>
+      </c>
+      <c r="E253" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B254" t="s">
+        <v>6</v>
+      </c>
+      <c r="D254" t="s">
+        <v>10</v>
+      </c>
+      <c r="E254" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B255" t="s">
+        <v>6</v>
+      </c>
+      <c r="D255" t="s">
+        <v>10</v>
+      </c>
+      <c r="E255" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B256" t="s">
+        <v>6</v>
+      </c>
+      <c r="D256" t="s">
+        <v>10</v>
+      </c>
+      <c r="E256" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B257" t="s">
+        <v>6</v>
+      </c>
+      <c r="D257" t="s">
+        <v>10</v>
+      </c>
+      <c r="E257" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B258" t="s">
+        <v>6</v>
+      </c>
+      <c r="D258" t="s">
+        <v>10</v>
+      </c>
+      <c r="E258" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A259" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B259" t="s">
+        <v>6</v>
+      </c>
+      <c r="D259" t="s">
+        <v>10</v>
+      </c>
+      <c r="E259" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B260" t="s">
+        <v>6</v>
+      </c>
+      <c r="D260" t="s">
+        <v>10</v>
+      </c>
+      <c r="E260" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B261" t="s">
+        <v>6</v>
+      </c>
+      <c r="D261" t="s">
+        <v>10</v>
+      </c>
+      <c r="E261" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B262" t="s">
+        <v>6</v>
+      </c>
+      <c r="D262" t="s">
+        <v>10</v>
+      </c>
+      <c r="E262" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B263" t="s">
+        <v>6</v>
+      </c>
+      <c r="D263" t="s">
+        <v>10</v>
+      </c>
+      <c r="E263" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B264" t="s">
+        <v>6</v>
+      </c>
+      <c r="D264" t="s">
+        <v>10</v>
+      </c>
+      <c r="E264" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B265" t="s">
+        <v>6</v>
+      </c>
+      <c r="D265" t="s">
+        <v>10</v>
+      </c>
+      <c r="E265" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B266" t="s">
+        <v>6</v>
+      </c>
+      <c r="D266" t="s">
+        <v>10</v>
+      </c>
+      <c r="E266" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B267" t="s">
+        <v>6</v>
+      </c>
+      <c r="C267" t="s">
+        <v>19</v>
+      </c>
+      <c r="D267" t="s">
+        <v>15</v>
+      </c>
+      <c r="E267" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B268" t="s">
+        <v>11</v>
+      </c>
+      <c r="C268" t="s">
+        <v>12</v>
+      </c>
+      <c r="D268" t="s">
+        <v>15</v>
+      </c>
+      <c r="E268" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B269" t="s">
+        <v>11</v>
+      </c>
+      <c r="C269" t="s">
+        <v>19</v>
+      </c>
+      <c r="D269" t="s">
+        <v>15</v>
+      </c>
+      <c r="E269" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B270" t="s">
+        <v>6</v>
+      </c>
+      <c r="C270" t="s">
+        <v>18</v>
+      </c>
+      <c r="D270" t="s">
+        <v>15</v>
+      </c>
+      <c r="E270" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D271" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D272" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D273" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D274" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B275" t="s">
+        <v>11</v>
+      </c>
+      <c r="C275" t="s">
+        <v>18</v>
+      </c>
+      <c r="D275" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added data from 3/25/2020
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFC3F3DF-13C0-1D43-84A0-5AED8A9D1873}"/>
+  <xr:revisionPtr revIDLastSave="407" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0DD2399-56DD-A540-9E52-39ACE1416E78}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25840" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>10-20</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Chambers</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Jackson</t>
   </si>
 </sst>
 </file>
@@ -959,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F275"/>
+  <dimension ref="A1:F365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D253" sqref="D253"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="D311" sqref="D311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2733,13 +2745,13 @@
         <v>43911</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C113" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -2747,13 +2759,16 @@
         <v>43911</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C114" t="s">
         <v>18</v>
       </c>
       <c r="D114" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="E114" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -2778,10 +2793,10 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -2789,13 +2804,13 @@
         <v>43911</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C117" t="s">
         <v>17</v>
       </c>
       <c r="D117" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -2806,7 +2821,7 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D118" t="s">
         <v>8</v>
@@ -2820,7 +2835,7 @@
         <v>11</v>
       </c>
       <c r="C119" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D119" t="s">
         <v>8</v>
@@ -2831,10 +2846,10 @@
         <v>43911</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D120" t="s">
         <v>8</v>
@@ -2848,10 +2863,10 @@
         <v>11</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -2859,13 +2874,13 @@
         <v>43911</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C122" t="s">
         <v>17</v>
       </c>
       <c r="D122" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -2873,10 +2888,10 @@
         <v>43911</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D123" t="s">
         <v>13</v>
@@ -2890,13 +2905,10 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D124" t="s">
-        <v>10</v>
-      </c>
-      <c r="E124" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -2904,16 +2916,13 @@
         <v>43911</v>
       </c>
       <c r="B125" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D125" t="s">
-        <v>10</v>
-      </c>
-      <c r="E125" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -2924,10 +2933,13 @@
         <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D126" t="s">
         <v>10</v>
+      </c>
+      <c r="E126" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -2938,13 +2950,13 @@
         <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D127" t="s">
         <v>10</v>
       </c>
       <c r="E127" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -2955,13 +2967,10 @@
         <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D128" t="s">
         <v>10</v>
-      </c>
-      <c r="E128" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -2972,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
@@ -2986,10 +2995,10 @@
         <v>43911</v>
       </c>
       <c r="B130" t="s">
-        <v>11</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C130" t="s">
+        <v>28</v>
       </c>
       <c r="D130" t="s">
         <v>10</v>
@@ -3006,13 +3015,13 @@
         <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D131" t="s">
         <v>10</v>
       </c>
       <c r="E131" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3020,13 +3029,16 @@
         <v>43911</v>
       </c>
       <c r="B132" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D132" t="s">
         <v>10</v>
+      </c>
+      <c r="E132" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -3034,10 +3046,10 @@
         <v>43911</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D133" t="s">
         <v>10</v>
@@ -3050,11 +3062,14 @@
       <c r="A134" s="1">
         <v>43911</v>
       </c>
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134" t="s">
+        <v>18</v>
+      </c>
       <c r="D134" t="s">
-        <v>30</v>
-      </c>
-      <c r="E134" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -3062,27 +3077,24 @@
         <v>43911</v>
       </c>
       <c r="B135" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D135" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="E135" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>43911</v>
       </c>
-      <c r="B136" t="s">
-        <v>11</v>
-      </c>
-      <c r="C136" t="s">
-        <v>19</v>
-      </c>
       <c r="D136" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E136" t="s">
         <v>9</v>
@@ -3096,13 +3108,10 @@
         <v>11</v>
       </c>
       <c r="C137" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D137" t="s">
-        <v>20</v>
-      </c>
-      <c r="E137" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -3110,24 +3119,30 @@
         <v>43911</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C138" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D138" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E138" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>43911</v>
       </c>
+      <c r="B139" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" t="s">
+        <v>12</v>
+      </c>
       <c r="D139" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E139" t="s">
         <v>9</v>
@@ -3137,14 +3152,17 @@
       <c r="A140" s="1">
         <v>43911</v>
       </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" t="s">
+        <v>18</v>
+      </c>
       <c r="D140" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E140" t="s">
-        <v>9</v>
-      </c>
-      <c r="F140" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3166,55 +3184,46 @@
         <v>22</v>
       </c>
       <c r="E142" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="F142" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>43911</v>
       </c>
-      <c r="B143" t="s">
-        <v>11</v>
-      </c>
-      <c r="C143" t="s">
-        <v>7</v>
-      </c>
       <c r="D143" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E143" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>43912</v>
-      </c>
-      <c r="B144" t="s">
-        <v>11</v>
-      </c>
-      <c r="C144" t="s">
-        <v>14</v>
+        <v>43911</v>
       </c>
       <c r="D144" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E144" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B145" t="s">
         <v>11</v>
       </c>
       <c r="C145" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D145" t="s">
-        <v>10</v>
-      </c>
-      <c r="E145" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -3222,16 +3231,16 @@
         <v>43912</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C146" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E146" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3239,10 +3248,10 @@
         <v>43912</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C147" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D147" t="s">
         <v>10</v>
@@ -3259,13 +3268,13 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D148" t="s">
         <v>10</v>
       </c>
       <c r="E148" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3293,13 +3302,13 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D150" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E150" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3307,16 +3316,16 @@
         <v>43912</v>
       </c>
       <c r="B151" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C151" t="s">
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E151" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3327,13 +3336,13 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D152" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E152" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -3341,13 +3350,13 @@
         <v>43912</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C153" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D153" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E153" t="s">
         <v>9</v>
@@ -3358,13 +3367,13 @@
         <v>43912</v>
       </c>
       <c r="B154" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D154" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E154" t="s">
         <v>16</v>
@@ -3375,24 +3384,30 @@
         <v>43912</v>
       </c>
       <c r="B155" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D155" t="s">
         <v>20</v>
       </c>
       <c r="E155" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>43912</v>
       </c>
+      <c r="B156" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" t="s">
+        <v>17</v>
+      </c>
       <c r="D156" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E156" t="s">
         <v>16</v>
@@ -3402,8 +3417,14 @@
       <c r="A157" s="1">
         <v>43912</v>
       </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>18</v>
+      </c>
       <c r="D157" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E157" t="s">
         <v>16</v>
@@ -3411,18 +3432,24 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="D158" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E158" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="D159" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E159" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -3517,31 +3544,16 @@
       <c r="A171" s="1">
         <v>43913</v>
       </c>
-      <c r="B171" t="s">
-        <v>6</v>
-      </c>
-      <c r="C171" t="s">
-        <v>12</v>
-      </c>
       <c r="D171" t="s">
-        <v>24</v>
-      </c>
-      <c r="E171" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>43913</v>
       </c>
-      <c r="B172" t="s">
-        <v>6</v>
-      </c>
-      <c r="C172" t="s">
-        <v>19</v>
-      </c>
       <c r="D172" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3549,16 +3561,16 @@
         <v>43913</v>
       </c>
       <c r="B173" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D173" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E173" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3566,16 +3578,13 @@
         <v>43913</v>
       </c>
       <c r="B174" t="s">
-        <v>11</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C174" t="s">
+        <v>19</v>
       </c>
       <c r="D174" t="s">
-        <v>15</v>
-      </c>
-      <c r="E174" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -3586,13 +3595,13 @@
         <v>11</v>
       </c>
       <c r="C175" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D175" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E175" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -3600,10 +3609,10 @@
         <v>43913</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
-      </c>
-      <c r="C176" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D176" t="s">
         <v>15</v>
@@ -3617,16 +3626,16 @@
         <v>43913</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C177" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D177" t="s">
         <v>15</v>
       </c>
       <c r="E177" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -3634,13 +3643,16 @@
         <v>43913</v>
       </c>
       <c r="B178" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D178" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="E178" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -3648,16 +3660,16 @@
         <v>43913</v>
       </c>
       <c r="B179" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C179" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D179" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E179" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -3665,16 +3677,13 @@
         <v>43913</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C180" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D180" t="s">
         <v>10</v>
-      </c>
-      <c r="E180" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -3685,10 +3694,10 @@
         <v>11</v>
       </c>
       <c r="C181" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D181" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E181" t="s">
         <v>16</v>
@@ -3705,7 +3714,10 @@
         <v>18</v>
       </c>
       <c r="D182" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="E182" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
@@ -3713,13 +3725,16 @@
         <v>43913</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C183" t="s">
         <v>17</v>
       </c>
       <c r="D183" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E183" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
@@ -3730,13 +3745,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D184" t="s">
-        <v>20</v>
-      </c>
-      <c r="E184" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -3750,10 +3762,7 @@
         <v>17</v>
       </c>
       <c r="D185" t="s">
-        <v>20</v>
-      </c>
-      <c r="E185" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
@@ -3764,7 +3773,7 @@
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D186" t="s">
         <v>20</v>
@@ -3781,7 +3790,7 @@
         <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D187" t="s">
         <v>20</v>
@@ -3798,7 +3807,7 @@
         <v>6</v>
       </c>
       <c r="C188" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D188" t="s">
         <v>20</v>
@@ -3812,19 +3821,16 @@
         <v>43913</v>
       </c>
       <c r="B189" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C189" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D189" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E189" t="s">
-        <v>16</v>
-      </c>
-      <c r="F189" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
@@ -3835,29 +3841,50 @@
         <v>6</v>
       </c>
       <c r="C190" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D190" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E190" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>43914</v>
+        <v>43913</v>
+      </c>
+      <c r="B191" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" t="s">
+        <v>17</v>
       </c>
       <c r="D191" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="E191" t="s">
+        <v>16</v>
+      </c>
+      <c r="F191" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>43914</v>
+        <v>43913</v>
+      </c>
+      <c r="B192" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" t="s">
+        <v>18</v>
       </c>
       <c r="D192" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="E192" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
@@ -3865,7 +3892,7 @@
         <v>43914</v>
       </c>
       <c r="D193" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -3873,7 +3900,7 @@
         <v>43914</v>
       </c>
       <c r="D194" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -3896,37 +3923,16 @@
       <c r="A197" s="1">
         <v>43914</v>
       </c>
-      <c r="B197" t="s">
-        <v>11</v>
-      </c>
-      <c r="C197" t="s">
-        <v>14</v>
-      </c>
       <c r="D197" t="s">
-        <v>24</v>
-      </c>
-      <c r="E197" t="s">
-        <v>16</v>
-      </c>
-      <c r="F197" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>43914</v>
       </c>
-      <c r="B198" t="s">
-        <v>11</v>
-      </c>
-      <c r="C198" t="s">
-        <v>14</v>
-      </c>
       <c r="D198" t="s">
-        <v>24</v>
-      </c>
-      <c r="E198" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
@@ -3937,7 +3943,7 @@
         <v>11</v>
       </c>
       <c r="C199" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D199" t="s">
         <v>24</v>
@@ -3945,6 +3951,9 @@
       <c r="E199" t="s">
         <v>16</v>
       </c>
+      <c r="F199" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
@@ -3954,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="C200" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D200" t="s">
         <v>24</v>
@@ -3976,8 +3985,8 @@
       <c r="D201" t="s">
         <v>24</v>
       </c>
-      <c r="F201" t="s">
-        <v>26</v>
+      <c r="E201" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -3988,13 +3997,13 @@
         <v>11</v>
       </c>
       <c r="C202" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D202" t="s">
         <v>24</v>
       </c>
-      <c r="F202" t="s">
-        <v>26</v>
+      <c r="E202" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
@@ -4004,8 +4013,8 @@
       <c r="B203" t="s">
         <v>11</v>
       </c>
-      <c r="C203" s="3" t="s">
-        <v>17</v>
+      <c r="C203" t="s">
+        <v>19</v>
       </c>
       <c r="D203" t="s">
         <v>24</v>
@@ -4022,20 +4031,23 @@
         <v>11</v>
       </c>
       <c r="C204" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D204" t="s">
         <v>24</v>
       </c>
+      <c r="F204" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>43914</v>
       </c>
       <c r="B205" t="s">
-        <v>6</v>
-      </c>
-      <c r="C205" t="s">
+        <v>11</v>
+      </c>
+      <c r="C205" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D205" t="s">
@@ -4053,10 +4065,10 @@
         <v>11</v>
       </c>
       <c r="C206" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D206" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
@@ -4064,13 +4076,16 @@
         <v>43914</v>
       </c>
       <c r="B207" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C207" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D207" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="F207" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
@@ -4084,10 +4099,7 @@
         <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>20</v>
-      </c>
-      <c r="E208" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -4098,13 +4110,10 @@
         <v>11</v>
       </c>
       <c r="C209" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D209" t="s">
-        <v>20</v>
-      </c>
-      <c r="E209" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -4112,7 +4121,7 @@
         <v>43914</v>
       </c>
       <c r="B210" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C210" t="s">
         <v>18</v>
@@ -4121,23 +4130,41 @@
         <v>20</v>
       </c>
       <c r="E210" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>43914</v>
       </c>
+      <c r="B211" t="s">
+        <v>11</v>
+      </c>
+      <c r="C211" t="s">
+        <v>17</v>
+      </c>
       <c r="D211" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="E211" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>43914</v>
       </c>
+      <c r="B212" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" t="s">
+        <v>18</v>
+      </c>
       <c r="D212" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="E212" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -4376,28 +4403,16 @@
       <c r="A242" s="1">
         <v>43914</v>
       </c>
-      <c r="B242" t="s">
-        <v>11</v>
-      </c>
       <c r="D242" t="s">
-        <v>10</v>
-      </c>
-      <c r="E242" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>43914</v>
       </c>
-      <c r="B243" t="s">
-        <v>11</v>
-      </c>
       <c r="D243" t="s">
-        <v>10</v>
-      </c>
-      <c r="E243" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
@@ -4439,7 +4454,7 @@
         <v>10</v>
       </c>
       <c r="E246" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -4453,7 +4468,7 @@
         <v>10</v>
       </c>
       <c r="E247" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -4467,7 +4482,7 @@
         <v>10</v>
       </c>
       <c r="E248" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -4481,7 +4496,7 @@
         <v>10</v>
       </c>
       <c r="E249" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -4531,7 +4546,7 @@
         <v>43914</v>
       </c>
       <c r="B253" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D253" t="s">
         <v>10</v>
@@ -4545,7 +4560,7 @@
         <v>43914</v>
       </c>
       <c r="B254" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D254" t="s">
         <v>10</v>
@@ -4729,14 +4744,11 @@
       <c r="B267" t="s">
         <v>6</v>
       </c>
-      <c r="C267" t="s">
-        <v>19</v>
-      </c>
       <c r="D267" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E267" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
@@ -4744,13 +4756,10 @@
         <v>43914</v>
       </c>
       <c r="B268" t="s">
-        <v>11</v>
-      </c>
-      <c r="C268" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D268" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E268" t="s">
         <v>16</v>
@@ -4761,7 +4770,7 @@
         <v>43914</v>
       </c>
       <c r="B269" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C269" t="s">
         <v>19</v>
@@ -4770,7 +4779,7 @@
         <v>15</v>
       </c>
       <c r="E269" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
@@ -4778,32 +4787,50 @@
         <v>43914</v>
       </c>
       <c r="B270" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C270" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D270" t="s">
         <v>15</v>
       </c>
       <c r="E270" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>43914</v>
       </c>
+      <c r="B271" t="s">
+        <v>11</v>
+      </c>
+      <c r="C271" t="s">
+        <v>19</v>
+      </c>
       <c r="D271" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="E271" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>43914</v>
       </c>
+      <c r="B272" t="s">
+        <v>6</v>
+      </c>
+      <c r="C272" t="s">
+        <v>18</v>
+      </c>
       <c r="D272" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="E272" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
@@ -4826,14 +4853,878 @@
       <c r="A275" s="1">
         <v>43914</v>
       </c>
-      <c r="B275" t="s">
-        <v>11</v>
-      </c>
-      <c r="C275" t="s">
+      <c r="D275" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>43914</v>
+      </c>
+      <c r="D276" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B277" t="s">
+        <v>11</v>
+      </c>
+      <c r="C277" t="s">
         <v>18</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D277" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B278" t="s">
+        <v>6</v>
+      </c>
+      <c r="C278" t="s">
+        <v>18</v>
+      </c>
+      <c r="D278" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B279" t="s">
+        <v>6</v>
+      </c>
+      <c r="C279" t="s">
+        <v>14</v>
+      </c>
+      <c r="D279" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B280" t="s">
+        <v>11</v>
+      </c>
+      <c r="C280" t="s">
+        <v>12</v>
+      </c>
+      <c r="D280" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D281" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D282" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D283" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D284" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D285" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D286" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D287" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D288" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B289" t="s">
+        <v>11</v>
+      </c>
+      <c r="C289" t="s">
+        <v>14</v>
+      </c>
+      <c r="D289" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B290" t="s">
+        <v>11</v>
+      </c>
+      <c r="C290" t="s">
+        <v>28</v>
+      </c>
+      <c r="D290" t="s">
+        <v>20</v>
+      </c>
+      <c r="E290" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B291" t="s">
+        <v>11</v>
+      </c>
+      <c r="C291" t="s">
+        <v>18</v>
+      </c>
+      <c r="D291" t="s">
+        <v>20</v>
+      </c>
+      <c r="E291" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B292" t="s">
+        <v>11</v>
+      </c>
+      <c r="C292" t="s">
+        <v>17</v>
+      </c>
+      <c r="D292" t="s">
+        <v>20</v>
+      </c>
+      <c r="E292" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293" t="s">
+        <v>18</v>
+      </c>
+      <c r="D293" t="s">
+        <v>20</v>
+      </c>
+      <c r="E293" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s">
+        <v>14</v>
+      </c>
+      <c r="D294" t="s">
+        <v>20</v>
+      </c>
+      <c r="E294" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D295" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D296" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D297" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D298" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D299" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D300" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D301" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D302" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D303" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D304" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D305" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D306" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D307" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D308" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D309" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D310" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D311" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D312" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A313" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D313" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A314" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D314" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A315" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D315" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D316" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D317" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D318" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A319" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D319" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D320" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A321" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D321" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D322" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D323" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D324" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D325" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D326" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D327" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D328" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D329" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D330" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D331" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D332" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D333" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D334" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B335" t="s">
+        <v>11</v>
+      </c>
+      <c r="C335" t="s">
+        <v>18</v>
+      </c>
+      <c r="D335" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B336" t="s">
+        <v>6</v>
+      </c>
+      <c r="C336" t="s">
+        <v>18</v>
+      </c>
+      <c r="D336" t="s">
+        <v>24</v>
+      </c>
+      <c r="F336" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B337" t="s">
+        <v>6</v>
+      </c>
+      <c r="C337" t="s">
+        <v>17</v>
+      </c>
+      <c r="D337" t="s">
+        <v>24</v>
+      </c>
+      <c r="F337" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B338" t="s">
+        <v>6</v>
+      </c>
+      <c r="C338" t="s">
+        <v>19</v>
+      </c>
+      <c r="D338" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A339" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B339" t="s">
+        <v>11</v>
+      </c>
+      <c r="C339" t="s">
+        <v>7</v>
+      </c>
+      <c r="D339" t="s">
+        <v>24</v>
+      </c>
+      <c r="E339" t="s">
+        <v>16</v>
+      </c>
+      <c r="F339" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A340" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D340" t="s">
+        <v>15</v>
+      </c>
+      <c r="E340" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A341" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D341" t="s">
+        <v>15</v>
+      </c>
+      <c r="E341" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A342" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D342" t="s">
+        <v>15</v>
+      </c>
+      <c r="E342" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A343" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D343" t="s">
+        <v>15</v>
+      </c>
+      <c r="E343" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A344" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D344" t="s">
+        <v>15</v>
+      </c>
+      <c r="E344" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A345" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D345" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A346" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D346" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A347" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D347" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A348" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D348" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A349" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D349" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A350" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D350" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A351" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D351" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D352" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A353" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D353" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A354" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D354" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A355" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D355" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A356" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D356" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A357" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D357" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A358" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D358" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A359" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D359" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A360" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D360" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A361" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D361" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A362" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D362" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A363" s="1">
+        <v>43915</v>
+      </c>
+      <c r="D363" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A364" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B364" t="s">
+        <v>6</v>
+      </c>
+      <c r="C364" t="s">
+        <v>14</v>
+      </c>
+      <c r="D364" t="s">
+        <v>20</v>
+      </c>
+      <c r="E364" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A365" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B365" t="s">
+        <v>11</v>
+      </c>
+      <c r="C365" t="s">
+        <v>14</v>
+      </c>
+      <c r="D365" t="s">
+        <v>21</v>
+      </c>
+      <c r="E365" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data from 3/26/2020
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0DD2399-56DD-A540-9E52-39ACE1416E78}"/>
+  <xr:revisionPtr revIDLastSave="426" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E93171A9-AAEA-2B4B-9CCD-A139BD36A3FB}"/>
   <bookViews>
-    <workbookView xWindow="25840" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="1140" windowWidth="50200" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Jackson</t>
+  </si>
+  <si>
+    <t>Walker</t>
   </si>
 </sst>
 </file>
@@ -971,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F365"/>
+  <dimension ref="A1:F456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="D311" sqref="D311"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="C439" sqref="C439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5727,6 +5730,734 @@
         <v>16</v>
       </c>
     </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A366" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D366" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A367" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D367" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A368" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D368" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A369" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D369" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A370" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D370" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A371" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D371" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A372" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D372" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A373" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D373" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A374" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D374" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A375" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D375" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A376" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D376" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A377" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D377" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A378" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D378" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A379" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D379" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A380" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D380" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A381" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D381" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A382" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D382" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A383" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D383" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A384" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D384" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A385" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D385" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A386" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D386" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A387" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D387" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D388" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A389" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D389" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A390" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D390" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A391" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D391" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A392" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D392" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A393" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D393" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A394" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D394" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A395" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D395" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A396" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D396" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A397" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D397" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A398" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D398" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A399" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D399" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A400" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D400" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A401" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D401" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A402" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D402" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A403" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D403" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A404" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D404" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A405" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D405" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A406" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D406" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A407" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D407" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A408" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D408" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A409" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D409" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A410" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D410" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A411" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D411" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A412" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D412" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A413" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D413" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A414" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D414" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A415" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D415" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A416" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D416" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A417" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D417" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A418" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D418" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A419" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D419" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A420" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D420" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A421" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D421" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A422" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D422" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A423" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D423" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A424" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D424" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A425" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D425" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A426" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D426" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A427" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D427" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A428" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D428" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A429" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D429" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A430" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D430" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A431" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D431" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A432" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D432" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D433" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D434" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D435" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D436" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D437" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D438" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D439" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D440" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D441" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D442" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D443" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D444" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D445" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D446" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D447" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D448" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A449" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D449" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A450" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D450" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A451" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D451" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A452" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D452" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A453" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D453" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A454" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D454" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A455" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D455" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A456" s="1">
+        <v>43916</v>
+      </c>
+      <c r="D456" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added data from 3/27/2020
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E93171A9-AAEA-2B4B-9CCD-A139BD36A3FB}"/>
+  <xr:revisionPtr revIDLastSave="463" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFA13782-1F2A-694E-BE9D-CF254FFD36CF}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1140" windowWidth="50200" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25840" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -974,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F456"/>
+  <dimension ref="A1:F530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="C439" sqref="C439"/>
+    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
+      <selection activeCell="C511" sqref="C511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6458,6 +6458,643 @@
         <v>22</v>
       </c>
     </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A457" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D457" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A458" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D458" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A459" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D459" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A460" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D460" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A461" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D461" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D462" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D463" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D464" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D465" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D466" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D467" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D468" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D469" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D470" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D471" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B472" t="s">
+        <v>11</v>
+      </c>
+      <c r="D472" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B473" t="s">
+        <v>11</v>
+      </c>
+      <c r="D473" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B474" t="s">
+        <v>11</v>
+      </c>
+      <c r="D474" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B475" t="s">
+        <v>11</v>
+      </c>
+      <c r="D475" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B476" t="s">
+        <v>11</v>
+      </c>
+      <c r="D476" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B477" t="s">
+        <v>11</v>
+      </c>
+      <c r="D477" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B478" t="s">
+        <v>11</v>
+      </c>
+      <c r="D478" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B479" t="s">
+        <v>11</v>
+      </c>
+      <c r="D479" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B480" t="s">
+        <v>6</v>
+      </c>
+      <c r="D480" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B481" t="s">
+        <v>6</v>
+      </c>
+      <c r="D481" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B482" t="s">
+        <v>6</v>
+      </c>
+      <c r="D482" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B483" t="s">
+        <v>6</v>
+      </c>
+      <c r="D483" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B484" t="s">
+        <v>6</v>
+      </c>
+      <c r="D484" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D485" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D486" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D487" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D488" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D489" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D490" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D491" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D492" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D493" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D494" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D495" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D496" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A497" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D497" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A498" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D498" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A499" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D499" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A500" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D500" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A501" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D501" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A502" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D502" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A503" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D503" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A504" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D504" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A505" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D505" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A506" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D506" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A507" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D507" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A508" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D508" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A509" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D509" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A510" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D510" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A511" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D511" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A512" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D512" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A513" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D513" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A514" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D514" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A515" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D515" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A516" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D516" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A517" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D517" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A518" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D518" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A519" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D519" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A520" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D520" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A521" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D521" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A522" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D522" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A523" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D523" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A524" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D524" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A525" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D525" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A526" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D526" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A527" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D527" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A528" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D528" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A529" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D529" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A530" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B530" t="s">
+        <v>11</v>
+      </c>
+      <c r="C530" t="s">
+        <v>18</v>
+      </c>
+      <c r="D530" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated data to 3/30/2020
</commit_message>
<xml_diff>
--- a/houstonNumbers.xlsx
+++ b/houstonNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd488cc0fec1f83/Python/Pandas/Houston Corona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="463" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFA13782-1F2A-694E-BE9D-CF254FFD36CF}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="113_{95FCC33E-C18B-2942-889B-B9F38780359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FD47BE2-F481-164D-AEAC-7A6DA8F752B8}"/>
   <bookViews>
-    <workbookView xWindow="25840" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="1140" windowWidth="24860" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houstonNumbers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Walker</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>Angelina</t>
   </si>
 </sst>
 </file>
@@ -974,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F530"/>
+  <dimension ref="A1:F1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
-      <selection activeCell="C511" sqref="C511"/>
+    <sheetView tabSelected="1" topLeftCell="A1035" workbookViewId="0">
+      <selection activeCell="A1081" sqref="A893:A1081"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7095,6 +7101,4615 @@
         <v>21</v>
       </c>
     </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A531" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D531" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A532" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D532" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A533" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D533" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A534" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D534" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A535" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D535" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A536" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D536" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A537" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D537" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A538" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D538" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A539" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D539" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A540" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D540" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A541" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D541" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A542" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D542" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A543" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D543" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A544" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D544" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A545" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D545" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A546" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D546" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A547" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D547" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A548" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D548" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A549" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D549" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A550" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D550" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A551" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D551" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A552" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D552" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A553" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D553" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A554" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D554" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A555" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D555" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A556" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D556" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A557" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D557" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A558" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D558" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A559" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D559" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A560" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D560" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A561" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D561" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A562" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D562" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A563" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D563" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A564" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D564" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A565" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D565" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A566" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D566" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A567" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D567" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A568" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D568" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A569" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D569" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A570" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D570" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A571" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D571" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A572" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D572" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A573" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D573" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A574" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D574" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A575" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D575" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A576" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D576" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A577" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D577" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A578" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D578" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A579" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D579" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A580" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D580" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A581" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D581" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A582" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D582" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A583" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D583" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A584" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D584" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A585" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D585" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A586" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D586" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A587" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D587" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A588" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D588" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A589" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D589" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A590" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D590" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A591" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D591" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A592" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D592" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A593" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D593" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A594" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D594" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A595" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D595" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A596" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D596" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A597" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D597" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A598" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D598" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A599" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D599" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A600" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D600" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="601" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A601" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D601" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A602" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D602" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="603" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A603" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D603" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A604" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D604" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A605" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D605" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A606" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D606" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A607" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D607" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A608" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D608" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A609" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D609" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A610" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D610" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A611" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D611" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A612" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D612" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A613" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D613" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A614" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D614" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A615" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D615" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A616" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D616" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A617" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D617" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A618" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D618" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A619" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D619" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A620" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D620" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A621" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D621" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A622" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D622" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A623" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D623" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A624" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D624" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A625" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D625" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A626" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D626" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A627" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D627" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A628" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D628" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A629" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D629" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A630" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D630" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A631" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D631" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A632" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D632" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A633" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D633" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="634" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A634" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D634" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A635" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D635" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A636" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D636" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A637" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D637" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A638" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D638" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A639" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D639" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A640" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D640" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A641" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D641" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A642" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D642" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A643" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D643" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A644" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D644" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A645" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D645" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A646" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D646" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A647" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D647" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A648" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D648" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A649" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D649" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A650" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D650" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A651" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D651" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A652" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D652" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A653" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D653" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A654" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D654" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A655" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D655" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A656" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D656" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A657" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D657" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A658" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D658" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="659" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A659" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D659" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A660" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D660" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A661" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D661" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A662" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D662" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A663" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D663" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A664" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D664" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A665" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D665" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A666" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D666" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A667" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D667" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A668" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D668" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A669" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D669" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A670" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D670" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A671" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D671" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A672" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D672" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="673" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A673" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D673" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="674" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A674" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D674" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="675" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A675" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D675" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="676" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A676" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D676" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A677" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D677" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="678" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A678" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D678" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A679" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D679" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="680" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A680" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D680" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="681" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A681" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D681" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="682" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A682" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D682" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="683" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A683" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D683" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="684" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A684" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D684" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="685" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A685" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D685" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="686" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A686" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D686" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="687" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A687" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D687" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="688" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A688" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D688" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A689" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D689" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A690" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D690" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A691" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D691" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A692" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D692" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A693" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D693" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A694" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D694" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A695" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D695" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A696" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D696" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A697" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D697" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A698" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D698" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A699" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D699" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A700" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D700" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A701" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D701" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="702" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A702" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D702" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A703" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D703" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A704" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D704" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A705" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D705" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A706" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D706" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A707" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D707" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A708" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D708" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="709" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A709" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D709" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A710" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D710" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="711" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A711" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D711" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A712" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D712" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A713" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D713" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A714" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D714" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A715" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D715" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A716" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D716" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A717" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D717" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A718" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D718" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A719" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D719" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A720" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D720" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A721" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D721" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="722" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A722" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D722" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A723" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D723" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A724" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D724" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="725" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A725" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D725" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="726" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A726" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D726" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A727" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D727" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="728" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A728" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D728" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="729" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A729" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D729" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A730" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D730" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="731" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A731" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D731" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A732" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D732" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A733" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D733" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A734" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D734" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A735" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D735" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A736" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D736" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A737" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D737" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="738" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A738" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D738" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="739" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A739" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D739" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="740" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A740" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D740" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="741" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A741" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D741" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="742" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A742" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D742" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A743" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D743" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="744" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A744" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D744" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="745" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A745" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D745" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="746" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A746" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D746" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="747" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A747" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D747" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="748" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A748" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D748" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="749" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A749" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D749" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="750" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A750" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D750" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="751" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A751" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D751" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="752" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A752" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D752" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="753" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A753" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D753" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="754" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A754" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D754" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="755" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A755" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D755" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="756" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A756" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D756" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="757" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A757" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D757" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="758" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A758" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D758" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="759" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A759" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D759" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="760" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A760" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D760" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="761" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A761" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D761" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="762" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A762" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D762" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="763" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A763" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D763" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="764" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A764" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D764" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="765" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A765" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D765" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A766" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D766" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="767" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A767" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D767" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A768" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D768" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A769" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D769" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="770" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A770" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D770" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A771" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D771" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A772" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D772" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="773" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A773" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D773" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A774" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D774" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A775" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D775" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="776" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A776" s="1">
+        <v>43918</v>
+      </c>
+      <c r="D776" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A777" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D777" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="778" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A778" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D778" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A779" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D779" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="780" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A780" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D780" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A781" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D781" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A782" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D782" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="783" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A783" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D783" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="784" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A784" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D784" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="785" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A785" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D785" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="786" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A786" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D786" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="787" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A787" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D787" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="788" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A788" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D788" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="789" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A789" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D789" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="790" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A790" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D790" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="791" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A791" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D791" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="792" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A792" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D792" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="793" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A793" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D793" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="794" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A794" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D794" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="795" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A795" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D795" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="796" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A796" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D796" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="797" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A797" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D797" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="798" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A798" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B798" t="s">
+        <v>11</v>
+      </c>
+      <c r="D798" t="s">
+        <v>20</v>
+      </c>
+      <c r="E798" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="799" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A799" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B799" t="s">
+        <v>11</v>
+      </c>
+      <c r="D799" t="s">
+        <v>20</v>
+      </c>
+      <c r="E799" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="800" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A800" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B800" t="s">
+        <v>11</v>
+      </c>
+      <c r="D800" t="s">
+        <v>20</v>
+      </c>
+      <c r="E800" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A801" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B801" t="s">
+        <v>11</v>
+      </c>
+      <c r="D801" t="s">
+        <v>20</v>
+      </c>
+      <c r="E801" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A802" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B802" t="s">
+        <v>11</v>
+      </c>
+      <c r="D802" t="s">
+        <v>20</v>
+      </c>
+      <c r="E802" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="803" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A803" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B803" t="s">
+        <v>11</v>
+      </c>
+      <c r="D803" t="s">
+        <v>20</v>
+      </c>
+      <c r="E803" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="804" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A804" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B804" t="s">
+        <v>11</v>
+      </c>
+      <c r="D804" t="s">
+        <v>20</v>
+      </c>
+      <c r="E804" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="805" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A805" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B805" t="s">
+        <v>6</v>
+      </c>
+      <c r="D805" t="s">
+        <v>20</v>
+      </c>
+      <c r="E805" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="806" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A806" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B806" t="s">
+        <v>6</v>
+      </c>
+      <c r="D806" t="s">
+        <v>20</v>
+      </c>
+      <c r="E806" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="807" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A807" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B807" t="s">
+        <v>6</v>
+      </c>
+      <c r="D807" t="s">
+        <v>20</v>
+      </c>
+      <c r="E807" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A808" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D808" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="809" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A809" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D809" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A810" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D810" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A811" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D811" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="812" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A812" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D812" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A813" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D813" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A814" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D814" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A815" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D815" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A816" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D816" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="817" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A817" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D817" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="818" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A818" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D818" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="819" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A819" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D819" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="820" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A820" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D820" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="821" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A821" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D821" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="822" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A822" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D822" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="823" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A823" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D823" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="824" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A824" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D824" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="825" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A825" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D825" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="826" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A826" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D826" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="827" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A827" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D827" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="828" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A828" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D828" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="829" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A829" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D829" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="830" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A830" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D830" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="831" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A831" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D831" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="832" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A832" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D832" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="833" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A833" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D833" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="834" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A834" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D834" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="835" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A835" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D835" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="836" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A836" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D836" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="837" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A837" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D837" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="838" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A838" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D838" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="839" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A839" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D839" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="840" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A840" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D840" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="841" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A841" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D841" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="842" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A842" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D842" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="843" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A843" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D843" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="844" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A844" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D844" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="845" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A845" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D845" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="846" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A846" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D846" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="847" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A847" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D847" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="848" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A848" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D848" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="849" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A849" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D849" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="850" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A850" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D850" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="851" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A851" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D851" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="852" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A852" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D852" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="853" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A853" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D853" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="854" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A854" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D854" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="855" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A855" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D855" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="856" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A856" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D856" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="857" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A857" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D857" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="858" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A858" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D858" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="859" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A859" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D859" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="860" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A860" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D860" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="861" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A861" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D861" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="862" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A862" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D862" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="863" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A863" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D863" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="864" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A864" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D864" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="865" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A865" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D865" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="866" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A866" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D866" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="867" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A867" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D867" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="868" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A868" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D868" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="869" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A869" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D869" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="870" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A870" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D870" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="871" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A871" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D871" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="872" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A872" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D872" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="873" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A873" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D873" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="874" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A874" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D874" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="875" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A875" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D875" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="876" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A876" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D876" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="877" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A877" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D877" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="878" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A878" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D878" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="879" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A879" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D879" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="880" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A880" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D880" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="881" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A881" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D881" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="882" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A882" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D882" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="883" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A883" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D883" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="884" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A884" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D884" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="885" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A885" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D885" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="886" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A886" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D886" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="887" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A887" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D887" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="888" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A888" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D888" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="889" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A889" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D889" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="890" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A890" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D890" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="891" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A891" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D891" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="892" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A892" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D892" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="893" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A893" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D893" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="894" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A894" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D894" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="895" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A895" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D895" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="896" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A896" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D896" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="897" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A897" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D897" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="898" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A898" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D898" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="899" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A899" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D899" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="900" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A900" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D900" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="901" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A901" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D901" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="902" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A902" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D902" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="903" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A903" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D903" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="904" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A904" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D904" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="905" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A905" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D905" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="906" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A906" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D906" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="907" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A907" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D907" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="908" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A908" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D908" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="909" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A909" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D909" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="910" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A910" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D910" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="911" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A911" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D911" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="912" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A912" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D912" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="913" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A913" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D913" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="914" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A914" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D914" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="915" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A915" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D915" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="916" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A916" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D916" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="917" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A917" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D917" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="918" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A918" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D918" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="919" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A919" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D919" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="920" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A920" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D920" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="921" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A921" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D921" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="922" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A922" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D922" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="923" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A923" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D923" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="924" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A924" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D924" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="925" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A925" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D925" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="926" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A926" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D926" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="927" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A927" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D927" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="928" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A928" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D928" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="929" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A929" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D929" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="930" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A930" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D930" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="931" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A931" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D931" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="932" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A932" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D932" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="933" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A933" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D933" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="934" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A934" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D934" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="935" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A935" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D935" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="936" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A936" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D936" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="937" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A937" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D937" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="938" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A938" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D938" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="939" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A939" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B939" t="s">
+        <v>11</v>
+      </c>
+      <c r="C939" t="s">
+        <v>14</v>
+      </c>
+      <c r="D939" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="940" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A940" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B940" t="s">
+        <v>11</v>
+      </c>
+      <c r="C940" t="s">
+        <v>17</v>
+      </c>
+      <c r="D940" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="941" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A941" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B941" t="s">
+        <v>6</v>
+      </c>
+      <c r="C941" t="s">
+        <v>7</v>
+      </c>
+      <c r="D941" t="s">
+        <v>24</v>
+      </c>
+      <c r="F941" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="942" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A942" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B942" t="s">
+        <v>11</v>
+      </c>
+      <c r="C942" t="s">
+        <v>17</v>
+      </c>
+      <c r="D942" t="s">
+        <v>24</v>
+      </c>
+      <c r="F942" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="943" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A943" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B943" t="s">
+        <v>6</v>
+      </c>
+      <c r="C943" t="s">
+        <v>17</v>
+      </c>
+      <c r="D943" t="s">
+        <v>24</v>
+      </c>
+      <c r="F943" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="944" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A944" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B944" t="s">
+        <v>6</v>
+      </c>
+      <c r="C944" t="s">
+        <v>7</v>
+      </c>
+      <c r="D944" t="s">
+        <v>24</v>
+      </c>
+      <c r="F944" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="945" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A945" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B945" t="s">
+        <v>6</v>
+      </c>
+      <c r="C945" t="s">
+        <v>28</v>
+      </c>
+      <c r="D945" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="946" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A946" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B946" t="s">
+        <v>11</v>
+      </c>
+      <c r="C946" t="s">
+        <v>28</v>
+      </c>
+      <c r="D946" t="s">
+        <v>24</v>
+      </c>
+      <c r="F946" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="947" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A947" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B947" t="s">
+        <v>6</v>
+      </c>
+      <c r="C947" t="s">
+        <v>18</v>
+      </c>
+      <c r="D947" t="s">
+        <v>24</v>
+      </c>
+      <c r="F947" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="948" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A948" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B948" t="s">
+        <v>6</v>
+      </c>
+      <c r="C948" t="s">
+        <v>17</v>
+      </c>
+      <c r="D948" t="s">
+        <v>24</v>
+      </c>
+      <c r="F948" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="949" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A949" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B949" t="s">
+        <v>6</v>
+      </c>
+      <c r="C949" t="s">
+        <v>19</v>
+      </c>
+      <c r="D949" t="s">
+        <v>24</v>
+      </c>
+      <c r="F949" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="950" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A950" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B950" t="s">
+        <v>6</v>
+      </c>
+      <c r="C950" t="s">
+        <v>7</v>
+      </c>
+      <c r="D950" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="951" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A951" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D951" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="952" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A952" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D952" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="953" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A953" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D953" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="954" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A954" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D954" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="955" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A955" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D955" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="956" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A956" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D956" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="957" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A957" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D957" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="958" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A958" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D958" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="959" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A959" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D959" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="960" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A960" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D960" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="961" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A961" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D961" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="962" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A962" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D962" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="963" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A963" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D963" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="964" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A964" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D964" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="965" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A965" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D965" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="966" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A966" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D966" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="967" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A967" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D967" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="968" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A968" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D968" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="969" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A969" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D969" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="970" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A970" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D970" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="971" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A971" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D971" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="972" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A972" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D972" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="973" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A973" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D973" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="974" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A974" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D974" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="975" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A975" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D975" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="976" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A976" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D976" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="977" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A977" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D977" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="978" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A978" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D978" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="979" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A979" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D979" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="980" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A980" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D980" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="981" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A981" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D981" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="982" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A982" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D982" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="983" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A983" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D983" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="984" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A984" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D984" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="985" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A985" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D985" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="986" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A986" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D986" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="987" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A987" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D987" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="988" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A988" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D988" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="989" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A989" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D989" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="990" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A990" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D990" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="991" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A991" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D991" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="992" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A992" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D992" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="993" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A993" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D993" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="994" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A994" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D994" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="995" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A995" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D995" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="996" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A996" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D996" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="997" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A997" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D997" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="998" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A998" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D998" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="999" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A999" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D999" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1000" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1001" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1002" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1003" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1004" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1005" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1006" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1007" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1008" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1009" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1010" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1011" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1012" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1013" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1014" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1015" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1016" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1017" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1018" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1019" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1020" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1021" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1022" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1023" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1024" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1025" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1026" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1032" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1032" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1033" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1033" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1034" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1035" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1036" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1037" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1038" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1039" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1040" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1041" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1042" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1043" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1044" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1045" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1046" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1047" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1048" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1049" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1050" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1051" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1052" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1053" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1054" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1055" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1056" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1057" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1058" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1059" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1060" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1061" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1062" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1063" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1064" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1065" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1066" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1067" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1068" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1069" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1070" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1071" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1072" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1073" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1074" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1076" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1077" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1078" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1079" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1080" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1081" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>